<commit_message>
changes new customer page utils and test class
</commit_message>
<xml_diff>
--- a/GitHubCheck/resources/demobank.xlsx
+++ b/GitHubCheck/resources/demobank.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="2280"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15945" windowHeight="6180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,19 +34,19 @@
     <t>vbgfty</t>
   </si>
   <si>
-    <t>hhjk44</t>
-  </si>
-  <si>
     <t>ujghjj</t>
   </si>
   <si>
-    <t>55ggg</t>
-  </si>
-  <si>
     <t>lkikkm</t>
   </si>
   <si>
-    <t>kkjk585</t>
+    <t>1345</t>
+  </si>
+  <si>
+    <t>kjhgff</t>
+  </si>
+  <si>
+    <t>78554</t>
   </si>
 </sst>
 </file>
@@ -82,8 +82,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,46 +374,47 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>1245</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created new scripts for excel data fetch, login scenarios, fetching data from excel for adding new customer
</commit_message>
<xml_diff>
--- a/GitHubCheck/resources/demobank.xlsx
+++ b/GitHubCheck/resources/demobank.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rages\git\DemoJavaProj\GitHubCheck\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D8898E-A76F-4006-9699-C7D1890B2D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15945" windowHeight="6180"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -47,12 +52,18 @@
   </si>
   <si>
     <t>78554</t>
+  </si>
+  <si>
+    <t>mngr434372</t>
+  </si>
+  <si>
+    <t>umAsapE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -364,16 +375,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -381,7 +392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -389,7 +400,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -397,7 +408,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -405,12 +416,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>